<commit_message>
Updated layout and added real product images
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,6 +427,9 @@
       <c r="H1" t="str">
         <v>disciplines</v>
       </c>
+      <c r="I1" t="str">
+        <v>instructor</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -560,9 +563,321 @@
         <v>Boxing, Wrestling, Jiu-Jitsu</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B8" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C8" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D8" t="str">
+        <v xml:space="preserve">I want to start A small MMA studio in my garage. I already have a small clientele base who is interested and instructors who would work for me. </v>
+      </c>
+      <c r="F8" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G8" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H8" t="str">
+        <v>MMA</v>
+      </c>
+      <c r="I8" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B9" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C9" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D9" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F9" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G9" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Wrestling</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B10" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C10" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D10" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F10" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G10" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B11" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C11" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D11" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F11" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G11" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B12" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C12" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D12" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F12" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G12" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H12" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B13" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C13" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D13" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F13" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G13" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H13" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B14" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C14" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D14" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F14" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H14" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B15" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C15" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D15" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F15" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G15" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B16" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C16" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D16" t="str">
+        <v>I want to start a big wrestling gym in a commercial area.</v>
+      </c>
+      <c r="F16" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G16" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="H16" t="str">
+        <v>Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Daniel</v>
+      </c>
+      <c r="B17" t="str">
+        <v>dansem@gnail.com</v>
+      </c>
+      <c r="C17" t="str">
+        <v>State college</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Gym</v>
+      </c>
+      <c r="F17" t="str">
+        <v>500-1000</v>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v>Muay Thai</v>
+      </c>
+      <c r="I17" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B18" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C18" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D18" t="str">
+        <v>MMA</v>
+      </c>
+      <c r="F18" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v>Muay Thai, Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I18" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Frank Roman Bevivino</v>
+      </c>
+      <c r="B19" t="str">
+        <v>frankbevivino@gmail.com</v>
+      </c>
+      <c r="C19" t="str">
+        <v>State College</v>
+      </c>
+      <c r="D19" t="str">
+        <v>MMA</v>
+      </c>
+      <c r="F19" t="str">
+        <v>1000-1500</v>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v>Muay Thai, Wrestling, Jiu-Jitsu</v>
+      </c>
+      <c r="I19" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>